<commit_message>
Honing Design Classes and Implementations
Rewrote design class IceCreamClientCommunication to reflect that the IceCreamClientCommunication subsystem of the icecreamserver sets message interfaces, starts server listening for messages, coordinates the server and an IceCreamProductRetrieval subsystem, and manages a ControllerToProcessIntoAnswer. Simplified the design class.

Simplified design class IceCreamProductRetrieval.

Exchanged Products.java for InfoAndProducts.java.

Exchanged SearchCriteria.java for SearchParameters.java.

Changed IceCreamClientCommunication.java to reflect corresponding design class in order of methods and sub-class. Put getSearchParameters in ControllerToProcessIntoAnswer.
</commit_message>
<xml_diff>
--- a/Interface_Design/System_Internal/Ice_Cream_Database_Design.xlsx
+++ b/Interface_Design/System_Internal/Ice_Cream_Database_Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\GitHub\Ice-Cream_Repository\Interface_Design\System_Internal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D945C8-84A8-46EC-B988-4D0745750429}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF13617-EE4E-4885-859E-D41765BD9A7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="70" windowWidth="18920" windowHeight="20780" xr2:uid="{D190C717-3E0B-4CF8-8987-9C797B15A2A4}"/>
+    <workbookView xWindow="19330" yWindow="80" windowWidth="18920" windowHeight="20780" xr2:uid="{D190C717-3E0B-4CF8-8987-9C797B15A2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -584,8 +584,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" customWidth="1"/>
-    <col min="2" max="2" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="14.1796875" customWidth="1"/>
     <col min="3" max="3" width="42.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -822,7 +822,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="53.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6328125" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.7265625" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>